<commit_message>
Changed dispalyed version. Published v1.4.
</commit_message>
<xml_diff>
--- a/Schematic/BOM_v2_0.xlsx
+++ b/Schematic/BOM_v2_0.xlsx
@@ -91,12 +91,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>MCP1702T</t>
-  </si>
-  <si>
-    <t>Linear voltage regulator</t>
-  </si>
-  <si>
     <t>DA1</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>MCP73831T-2ATI/OT</t>
+  </si>
+  <si>
+    <t>MCP1702T-3302</t>
+  </si>
+  <si>
+    <t>Linear voltage regulator 3.3V</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="36.21875" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" customWidth="1"/>
   </cols>
@@ -612,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3">
         <v>7</v>
@@ -629,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -708,7 +708,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>19</v>
@@ -739,16 +739,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -756,16 +756,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -773,16 +773,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -790,16 +790,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -807,16 +807,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -824,16 +824,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -841,16 +841,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
@@ -858,16 +858,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="3">
         <v>4</v>
@@ -875,16 +875,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -892,16 +892,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -909,16 +909,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>

</xml_diff>